<commit_message>
Updated all_join.csv to add unique ids to points that were manually added
</commit_message>
<xml_diff>
--- a/data/nyc_data_join.xlsx
+++ b/data/nyc_data_join.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64426d83357dbd62/LHL/_DataScienciBootCamp/Midterm_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2423" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{157B2C16-1E67-45E5-852F-65DCE19EA009}"/>
+  <xr:revisionPtr revIDLastSave="2471" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2EC2AA-00F4-43C9-9E11-CD163A72A185}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C1537D77-E0D5-2B49-9CF0-C1029E12ACBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C1537D77-E0D5-2B49-9CF0-C1029E12ACBF}"/>
   </bookViews>
   <sheets>
     <sheet name="housing_prices" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5408" uniqueCount="1028">
   <si>
     <t>Astoria</t>
   </si>
@@ -3133,6 +3133,9 @@
   </si>
   <si>
     <t>Central Harlem === Herlem == west Harlam</t>
+  </si>
+  <si>
+    <t>S &gt; BR_1</t>
   </si>
 </sst>
 </file>
@@ -3140,7 +3143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -3199,7 +3202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3242,6 +3245,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3271,7 +3280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3293,18 +3302,61 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3605,22 +3657,22 @@
     <sortCondition ref="B1:B56"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D9345F85-8022-4F46-AE6A-DC139A4E6A64}" uniqueName="1" name="borough" queryTableFieldId="1" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{A0C7E5AD-E299-4DE5-BE00-487E15EAA7F5}" uniqueName="2" name="neigborhood" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{47D42903-B069-47AD-BFDC-28D172D7D3D6}" uniqueName="3" name="studio" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{D9345F85-8022-4F46-AE6A-DC139A4E6A64}" uniqueName="1" name="borough" queryTableFieldId="1" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{A0C7E5AD-E299-4DE5-BE00-487E15EAA7F5}" uniqueName="2" name="neigborhood" queryTableFieldId="2" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{47D42903-B069-47AD-BFDC-28D172D7D3D6}" uniqueName="3" name="studio" queryTableFieldId="3" dataDxfId="44"/>
     <tableColumn id="4" xr3:uid="{589D20F3-F2C9-4552-B53E-6B3C15607475}" uniqueName="4" name="1_bedroom" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{E21E2E8D-1B2D-48C4-AE50-0A1255BC4B80}" uniqueName="5" name="2_bedroom" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{2E64E790-61AE-4948-B9F0-3F46369158F4}" uniqueName="6" name="3_bedroom" queryTableFieldId="6" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{7E3BE24A-A11E-40FB-803B-0B880F1FA722}" uniqueName="7" name="studio2" queryTableFieldId="7" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{2E64E790-61AE-4948-B9F0-3F46369158F4}" uniqueName="6" name="3_bedroom" queryTableFieldId="6" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{7E3BE24A-A11E-40FB-803B-0B880F1FA722}" uniqueName="7" name="studio2" queryTableFieldId="7" dataDxfId="42">
       <calculatedColumnFormula>nyc_housing_prices_jul_2020[[#This Row],[studio]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3B433734-4DB6-45F6-8A40-D89E5B35E594}" uniqueName="8" name="1_bedroom3" queryTableFieldId="8" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{3B433734-4DB6-45F6-8A40-D89E5B35E594}" uniqueName="8" name="1_bedroom3" queryTableFieldId="8" dataDxfId="41">
       <calculatedColumnFormula>nyc_housing_prices_jul_2020[[#This Row],[1_bedroom]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{658DBF81-BBCA-45E3-AB66-FFE2C61D4932}" uniqueName="9" name="2_bedroom4" queryTableFieldId="9" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{658DBF81-BBCA-45E3-AB66-FFE2C61D4932}" uniqueName="9" name="2_bedroom4" queryTableFieldId="9" dataDxfId="40">
       <calculatedColumnFormula>nyc_housing_prices_jul_2020[[#This Row],[2_bedroom]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{77C4B9DF-55D2-412B-B276-11C8659862C5}" uniqueName="10" name="3_bedroom5" queryTableFieldId="10" dataDxfId="33">
+    <tableColumn id="10" xr3:uid="{77C4B9DF-55D2-412B-B276-11C8659862C5}" uniqueName="10" name="3_bedroom5" queryTableFieldId="10" dataDxfId="39">
       <calculatedColumnFormula>nyc_housing_prices_jul_2020[[#This Row],[3_bedroom]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8105,7 +8157,7 @@
         <v>157</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C139" si="6">B131*1</f>
+        <f t="shared" ref="C131:C138" si="6">B131*1</f>
         <v>1650</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -12820,8 +12872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEB5DD7-7FD4-4372-9473-5927F35A1625}">
   <dimension ref="A1:O287"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21415,112 +21467,112 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576 M1:M1048576 J1:J1048576">
-    <cfRule type="cellIs" dxfId="32" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="103" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="111" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="112" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52">
-    <cfRule type="cellIs" dxfId="29" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="94" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="95" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="96" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54">
-    <cfRule type="cellIs" dxfId="26" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="91" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="92" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="93" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M55">
-    <cfRule type="cellIs" dxfId="23" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="88" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="89" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="90" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M79:M92">
-    <cfRule type="cellIs" dxfId="20" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="79" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="80" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="81" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M138:M144">
-    <cfRule type="cellIs" dxfId="17" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="64" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="65" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="66" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M145:M169">
-    <cfRule type="cellIs" dxfId="14" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="49" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="50" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="51" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M170">
-    <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="37" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="38" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="39" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M189:M205">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M206:M233">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21532,8 +21584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7463727-FBA3-4F81-8943-39D6D8A4844B}">
   <dimension ref="A1:R243"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="J237" sqref="J237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21586,6 +21638,9 @@
       <c r="J1" t="s">
         <v>590</v>
       </c>
+      <c r="M1" t="s">
+        <v>1027</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -21612,7 +21667,7 @@
         <f>IF(AND(E2&gt;0,I2&gt;0),I2-E2,0)</f>
         <v>0</v>
       </c>
-      <c r="M2" t="b">
+      <c r="M2" s="12" t="b">
         <f>IF(G2&gt;H2,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -21636,7 +21691,7 @@
         <f t="shared" ref="L3:L66" si="2">IF(AND(E3&gt;0,I3&gt;0),I3-E3,0)</f>
         <v>0</v>
       </c>
-      <c r="M3" t="b">
+      <c r="M3" s="12" t="b">
         <f t="shared" ref="M3:M66" si="3">IF(G3&gt;H3,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -21660,7 +21715,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M4" t="b">
+      <c r="M4" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21690,7 +21745,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M5" t="b">
+      <c r="M5" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21720,7 +21775,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" t="b">
+      <c r="M6" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -21738,19 +21793,19 @@
       <c r="I7" s="16">
         <v>1825</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" t="b">
+      <c r="M7" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -21795,7 +21850,7 @@
         <f t="shared" si="2"/>
         <v>-2428</v>
       </c>
-      <c r="M8" t="b">
+      <c r="M8" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21825,7 +21880,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" t="b">
+      <c r="M9" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -21855,7 +21910,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" t="b">
+      <c r="M10" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21885,7 +21940,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M11" t="b">
+      <c r="M11" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21930,7 +21985,7 @@
         <f t="shared" si="2"/>
         <v>-411</v>
       </c>
-      <c r="M12" t="b">
+      <c r="M12" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21966,7 +22021,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M13" t="b">
+      <c r="M13" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -21993,7 +22048,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M14" t="b">
+      <c r="M14" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22020,7 +22075,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M15" t="b">
+      <c r="M15" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22038,19 +22093,19 @@
       <c r="I16" s="16">
         <v>1795</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" t="b">
+      <c r="M16" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -22077,7 +22132,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M17" t="b">
+      <c r="M17" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22104,7 +22159,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" t="b">
+      <c r="M18" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22149,7 +22204,7 @@
         <f t="shared" si="2"/>
         <v>-1606</v>
       </c>
-      <c r="M19" t="b">
+      <c r="M19" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -22179,7 +22234,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M20" t="b">
+      <c r="M20" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22215,7 +22270,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M21" t="b">
+      <c r="M21" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22245,7 +22300,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M22" t="b">
+      <c r="M22" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22275,7 +22330,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M23" t="b">
+      <c r="M23" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22305,7 +22360,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M24" t="b">
+      <c r="M24" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22332,7 +22387,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M25" t="b">
+      <c r="M25" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22377,7 +22432,7 @@
         <f t="shared" si="2"/>
         <v>-2533</v>
       </c>
-      <c r="M26" t="b">
+      <c r="M26" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22407,7 +22462,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M27" t="b">
+      <c r="M27" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22431,7 +22486,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M28" t="b">
+      <c r="M28" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22449,19 +22504,19 @@
       <c r="I29" s="16">
         <v>1888</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M29" t="b">
+      <c r="M29" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -22488,7 +22543,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M30" t="b">
+      <c r="M30" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22533,7 +22588,7 @@
         <f t="shared" si="2"/>
         <v>-649</v>
       </c>
-      <c r="M31" t="b">
+      <c r="M31" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22563,7 +22618,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M32" t="b">
+      <c r="M32" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -22599,7 +22654,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M33" t="b">
+      <c r="M33" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22644,7 +22699,7 @@
         <f t="shared" si="2"/>
         <v>-914</v>
       </c>
-      <c r="M34" t="b">
+      <c r="M34" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22668,7 +22723,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M35" t="b">
+      <c r="M35" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22692,7 +22747,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M36" t="b">
+      <c r="M36" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22722,7 +22777,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M37" t="b">
+      <c r="M37" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22767,7 +22822,7 @@
         <f t="shared" si="2"/>
         <v>-3941</v>
       </c>
-      <c r="M38" t="b">
+      <c r="M38" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22812,7 +22867,7 @@
         <f t="shared" si="2"/>
         <v>-2038</v>
       </c>
-      <c r="M39" t="b">
+      <c r="M39" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22842,7 +22897,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M40" t="b">
+      <c r="M40" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -22869,7 +22924,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M41" t="b">
+      <c r="M41" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22899,7 +22954,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M42" t="b">
+      <c r="M42" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22929,7 +22984,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M43" t="b">
+      <c r="M43" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -22959,7 +23014,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M44" t="b">
+      <c r="M44" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23004,7 +23059,7 @@
         <f t="shared" si="2"/>
         <v>-500</v>
       </c>
-      <c r="M45" t="b">
+      <c r="M45" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23049,7 +23104,7 @@
         <f t="shared" si="2"/>
         <v>-1522</v>
       </c>
-      <c r="M46" t="b">
+      <c r="M46" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23076,7 +23131,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M47" t="b">
+      <c r="M47" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23103,7 +23158,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M48" t="b">
+      <c r="M48" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23133,7 +23188,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M49" t="b">
+      <c r="M49" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23163,7 +23218,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M50" t="b">
+      <c r="M50" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23193,7 +23248,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M51" t="b">
+      <c r="M51" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23217,7 +23272,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M52" t="b">
+      <c r="M52" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23235,19 +23290,19 @@
       <c r="I53" s="16">
         <v>1950</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M53" t="b">
+      <c r="M53" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23271,7 +23326,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M54" t="b">
+      <c r="M54" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23295,7 +23350,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M55" t="b">
+      <c r="M55" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23340,7 +23395,7 @@
         <f t="shared" si="2"/>
         <v>-382</v>
       </c>
-      <c r="M56" t="b">
+      <c r="M56" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23367,7 +23422,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M57" t="b">
+      <c r="M57" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23394,7 +23449,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M58" t="b">
+      <c r="M58" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23424,7 +23479,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M59" t="b">
+      <c r="M59" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23469,7 +23524,7 @@
         <f t="shared" si="2"/>
         <v>-491</v>
       </c>
-      <c r="M60" t="b">
+      <c r="M60" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23514,7 +23569,7 @@
         <f t="shared" si="2"/>
         <v>-191</v>
       </c>
-      <c r="M61" t="b">
+      <c r="M61" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23544,7 +23599,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M62" t="b">
+      <c r="M62" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23571,7 +23626,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M63" t="b">
+      <c r="M63" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23601,7 +23656,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M64" t="b">
+      <c r="M64" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23646,7 +23701,7 @@
         <f t="shared" si="2"/>
         <v>-968</v>
       </c>
-      <c r="M65" t="b">
+      <c r="M65" s="12" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -23676,7 +23731,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M66" t="b">
+      <c r="M66" s="12" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -23700,7 +23755,7 @@
         <f t="shared" ref="L67:L130" si="6">IF(AND(E67&gt;0,I67&gt;0),I67-E67,0)</f>
         <v>0</v>
       </c>
-      <c r="M67" t="b">
+      <c r="M67" s="12" t="b">
         <f t="shared" ref="M67:M130" si="7">IF(G67&gt;H67,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -23745,7 +23800,7 @@
         <f t="shared" si="6"/>
         <v>-1111</v>
       </c>
-      <c r="M68" t="b">
+      <c r="M68" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -23775,7 +23830,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M69" t="b">
+      <c r="M69" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -23802,7 +23857,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M70" t="b">
+      <c r="M70" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -23832,7 +23887,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M71" t="b">
+      <c r="M71" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -23877,7 +23932,7 @@
         <f t="shared" si="6"/>
         <v>-2415</v>
       </c>
-      <c r="M72" t="b">
+      <c r="M72" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -23895,19 +23950,19 @@
       <c r="I73" s="16">
         <v>2117</v>
       </c>
-      <c r="J73" s="11">
+      <c r="J73" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K73" s="11">
+      <c r="K73" s="25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L73" s="11">
+      <c r="L73" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M73" t="b">
+      <c r="M73" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -23937,7 +23992,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M74" t="b">
+      <c r="M74" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -23973,7 +24028,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M75" t="b">
+      <c r="M75" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24003,7 +24058,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M76" t="b">
+      <c r="M76" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24027,7 +24082,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M77" t="b">
+      <c r="M77" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24057,7 +24112,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M78" t="b">
+      <c r="M78" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24087,7 +24142,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M79" t="b">
+      <c r="M79" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24117,7 +24172,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M80" t="b">
+      <c r="M80" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24147,7 +24202,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M81" t="b">
+      <c r="M81" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24177,7 +24232,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M82" t="b">
+      <c r="M82" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24207,7 +24262,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M83" t="b">
+      <c r="M83" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24252,7 +24307,7 @@
         <f t="shared" si="6"/>
         <v>-1213</v>
       </c>
-      <c r="M84" t="b">
+      <c r="M84" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24279,7 +24334,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M85" t="b">
+      <c r="M85" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24309,7 +24364,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M86" t="b">
+      <c r="M86" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24336,7 +24391,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M87" t="b">
+      <c r="M87" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24366,7 +24421,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M88" t="b">
+      <c r="M88" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24390,7 +24445,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M89" t="b">
+      <c r="M89" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24417,7 +24472,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M90" t="b">
+      <c r="M90" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24447,7 +24502,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M91" t="b">
+      <c r="M91" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24492,7 +24547,7 @@
         <f t="shared" si="6"/>
         <v>-1238</v>
       </c>
-      <c r="M92" t="b">
+      <c r="M92" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24537,7 +24592,7 @@
         <f t="shared" si="6"/>
         <v>-1783</v>
       </c>
-      <c r="M93" t="b">
+      <c r="M93" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24561,7 +24616,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M94" t="b">
+      <c r="M94" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24585,7 +24640,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M95" t="b">
+      <c r="M95" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24615,7 +24670,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M96" t="b">
+      <c r="M96" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24642,7 +24697,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M97" t="b">
+      <c r="M97" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24687,7 +24742,7 @@
         <f t="shared" si="6"/>
         <v>-1158</v>
       </c>
-      <c r="M98" t="b">
+      <c r="M98" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24732,7 +24787,7 @@
         <f t="shared" si="6"/>
         <v>-3500</v>
       </c>
-      <c r="M99" t="b">
+      <c r="M99" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24750,19 +24805,19 @@
       <c r="I100" s="16">
         <v>2100</v>
       </c>
-      <c r="J100">
+      <c r="J100" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K100">
+      <c r="K100" s="11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L100">
+      <c r="L100" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M100" t="b">
+      <c r="M100" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -24786,7 +24841,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M101" t="b">
+      <c r="M101" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24822,7 +24877,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M102" t="b">
+      <c r="M102" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24858,7 +24913,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M103" t="b">
+      <c r="M103" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24888,7 +24943,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M104" t="b">
+      <c r="M104" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24918,7 +24973,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M105" t="b">
+      <c r="M105" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24945,7 +25000,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M106" t="b">
+      <c r="M106" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24972,7 +25027,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M107" t="b">
+      <c r="M107" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -24999,7 +25054,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M108" t="b">
+      <c r="M108" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25029,7 +25084,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M109" t="b">
+      <c r="M109" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25053,7 +25108,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M110" t="b">
+      <c r="M110" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25080,7 +25135,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M111" t="b">
+      <c r="M111" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25125,7 +25180,7 @@
         <f t="shared" si="6"/>
         <v>-173</v>
       </c>
-      <c r="M112" t="b">
+      <c r="M112" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25155,7 +25210,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M113" t="b">
+      <c r="M113" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25185,7 +25240,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M114" t="b">
+      <c r="M114" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25215,7 +25270,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M115" t="b">
+      <c r="M115" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25245,7 +25300,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M116" t="b">
+      <c r="M116" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25290,7 +25345,7 @@
         <f t="shared" si="6"/>
         <v>-802</v>
       </c>
-      <c r="M117" t="b">
+      <c r="M117" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25320,7 +25375,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M118" t="b">
+      <c r="M118" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25350,7 +25405,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M119" t="b">
+      <c r="M119" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25368,19 +25423,19 @@
       <c r="I120" s="16">
         <v>2198</v>
       </c>
-      <c r="J120">
+      <c r="J120" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K120">
+      <c r="K120" s="11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L120">
+      <c r="L120" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M120" t="b">
+      <c r="M120" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -25410,7 +25465,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M121" t="b">
+      <c r="M121" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25440,7 +25495,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M122" t="b">
+      <c r="M122" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25458,19 +25513,19 @@
       <c r="I123" s="16">
         <v>2000</v>
       </c>
-      <c r="J123" s="11">
+      <c r="J123" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K123" s="11">
+      <c r="K123" s="25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L123" s="11">
+      <c r="L123" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M123" t="b">
+      <c r="M123" s="12" t="b">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -25506,7 +25561,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M124" t="b">
+      <c r="M124" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25548,7 +25603,7 @@
         <f t="shared" si="6"/>
         <v>-983</v>
       </c>
-      <c r="M125" t="b">
+      <c r="M125" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25584,7 +25639,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M126" t="b">
+      <c r="M126" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25611,7 +25666,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M127" t="b">
+      <c r="M127" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25641,7 +25696,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M128" t="b">
+      <c r="M128" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25665,7 +25720,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M129" t="b">
+      <c r="M129" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25710,7 +25765,7 @@
         <f t="shared" si="6"/>
         <v>-1504</v>
       </c>
-      <c r="M130" t="b">
+      <c r="M130" s="12" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -25728,19 +25783,19 @@
       <c r="I131" s="16">
         <v>2250</v>
       </c>
-      <c r="J131">
+      <c r="J131" s="11">
         <f t="shared" ref="J131:J194" si="8">IF(AND(C131&gt;0,G131&gt;0),G131-C131,0)</f>
         <v>0</v>
       </c>
-      <c r="K131">
+      <c r="K131" s="11">
         <f t="shared" ref="K131:K194" si="9">IF(AND(D131&gt;0,H131&gt;0),H131-D131,0)</f>
         <v>0</v>
       </c>
-      <c r="L131">
+      <c r="L131" s="11">
         <f t="shared" ref="L131:L194" si="10">IF(AND(E131&gt;0,I131&gt;0),I131-E131,0)</f>
         <v>0</v>
       </c>
-      <c r="M131" t="b">
+      <c r="M131" s="12" t="b">
         <f t="shared" ref="M131:M194" si="11">IF(G131&gt;H131,TRUE,FALSE)</f>
         <v>1</v>
       </c>
@@ -25767,7 +25822,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M132" t="b">
+      <c r="M132" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25794,7 +25849,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M133" t="b">
+      <c r="M133" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25821,7 +25876,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M134" t="b">
+      <c r="M134" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25848,7 +25903,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M135" t="b">
+      <c r="M135" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25878,7 +25933,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M136" t="b">
+      <c r="M136" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -25905,7 +25960,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M137" t="b">
+      <c r="M137" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25932,7 +25987,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M138" t="b">
+      <c r="M138" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -25956,7 +26011,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M139" t="b">
+      <c r="M139" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26001,7 +26056,7 @@
         <f t="shared" si="10"/>
         <v>-2111</v>
       </c>
-      <c r="M140" t="b">
+      <c r="M140" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26037,7 +26092,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M141" t="b">
+      <c r="M141" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26067,7 +26122,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M142" t="b">
+      <c r="M142" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26091,7 +26146,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M143" t="b">
+      <c r="M143" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26127,7 +26182,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M144" t="b">
+      <c r="M144" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26157,7 +26212,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M145" t="b">
+      <c r="M145" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26187,7 +26242,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M146" t="b">
+      <c r="M146" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26211,7 +26266,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M147" t="b">
+      <c r="M147" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26241,7 +26296,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M148" t="b">
+      <c r="M148" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26271,7 +26326,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M149" t="b">
+      <c r="M149" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26301,7 +26356,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M150" t="b">
+      <c r="M150" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26346,7 +26401,7 @@
         <f t="shared" si="10"/>
         <v>25</v>
       </c>
-      <c r="M151" t="b">
+      <c r="M151" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26370,7 +26425,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M152" t="b">
+      <c r="M152" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26397,7 +26452,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M153" t="b">
+      <c r="M153" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26424,7 +26479,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M154" t="b">
+      <c r="M154" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26469,7 +26524,7 @@
         <f t="shared" si="10"/>
         <v>-2430</v>
       </c>
-      <c r="M155" t="b">
+      <c r="M155" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26514,7 +26569,7 @@
         <f t="shared" si="10"/>
         <v>-1333</v>
       </c>
-      <c r="M156" t="b">
+      <c r="M156" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26544,7 +26599,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M157" t="b">
+      <c r="M157" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26562,19 +26617,19 @@
       <c r="I158" s="16">
         <v>1895</v>
       </c>
-      <c r="J158">
+      <c r="J158" s="11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K158">
+      <c r="K158" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L158">
+      <c r="L158" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M158" t="b">
+      <c r="M158" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26601,7 +26656,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M159" t="b">
+      <c r="M159" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26631,7 +26686,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M160" t="b">
+      <c r="M160" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26649,19 +26704,19 @@
       <c r="I161" s="16">
         <v>2100</v>
       </c>
-      <c r="J161">
+      <c r="J161" s="11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K161">
+      <c r="K161" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L161">
+      <c r="L161" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M161" t="b">
+      <c r="M161" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26694,19 +26749,19 @@
       <c r="I162" s="16">
         <v>2700</v>
       </c>
-      <c r="J162">
+      <c r="J162" s="11">
         <f t="shared" si="8"/>
         <v>-295</v>
       </c>
-      <c r="K162">
+      <c r="K162" s="11">
         <f t="shared" si="9"/>
         <v>-264</v>
       </c>
-      <c r="L162">
+      <c r="L162" s="11">
         <f t="shared" si="10"/>
         <v>-722</v>
       </c>
-      <c r="M162" t="b">
+      <c r="M162" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26736,7 +26791,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M163" t="b">
+      <c r="M163" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26772,7 +26827,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M164" t="b">
+      <c r="M164" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26790,19 +26845,19 @@
       <c r="I165" s="16">
         <v>1950</v>
       </c>
-      <c r="J165">
+      <c r="J165" s="11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K165">
+      <c r="K165" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L165">
+      <c r="L165" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M165" t="b">
+      <c r="M165" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26826,7 +26881,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M166" t="b">
+      <c r="M166" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26844,19 +26899,19 @@
       <c r="I167" s="16">
         <v>2150</v>
       </c>
-      <c r="J167">
+      <c r="J167" s="11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K167">
+      <c r="K167" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L167">
+      <c r="L167" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M167" t="b">
+      <c r="M167" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -26883,7 +26938,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M168" t="b">
+      <c r="M168" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26907,7 +26962,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M169" t="b">
+      <c r="M169" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26952,7 +27007,7 @@
         <f t="shared" si="10"/>
         <v>-921</v>
       </c>
-      <c r="M170" t="b">
+      <c r="M170" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -26988,7 +27043,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M171" t="b">
+      <c r="M171" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27018,7 +27073,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M172" t="b">
+      <c r="M172" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27036,19 +27091,19 @@
       <c r="I173" s="16">
         <v>2000</v>
       </c>
-      <c r="J173">
+      <c r="J173" s="25">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K173">
+      <c r="K173" s="25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L173">
+      <c r="L173" s="25">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M173" t="b">
+      <c r="M173" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -27060,17 +27115,11 @@
       <c r="B174" t="s">
         <v>155</v>
       </c>
-      <c r="C174" s="12">
-        <v>-9999</v>
-      </c>
       <c r="D174" s="15">
         <v>2300</v>
       </c>
       <c r="E174" s="16">
         <v>4287</v>
-      </c>
-      <c r="F174" s="13">
-        <v>-9999</v>
       </c>
       <c r="G174" s="12">
         <v>1673</v>
@@ -27093,7 +27142,7 @@
         <f t="shared" si="10"/>
         <v>-1887</v>
       </c>
-      <c r="M174" t="b">
+      <c r="M174" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27123,7 +27172,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M175" t="b">
+      <c r="M175" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27141,19 +27190,19 @@
       <c r="I176" s="16">
         <v>1980</v>
       </c>
-      <c r="J176">
+      <c r="J176" s="11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K176">
+      <c r="K176" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L176">
+      <c r="L176" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M176" t="b">
+      <c r="M176" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -27183,7 +27232,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M177" t="b">
+      <c r="M177" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27213,7 +27262,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M178" t="b">
+      <c r="M178" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27249,7 +27298,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M179" t="b">
+      <c r="M179" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27273,7 +27322,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M180" t="b">
+      <c r="M180" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27291,19 +27340,19 @@
       <c r="I181" s="16">
         <v>2000</v>
       </c>
-      <c r="J181">
+      <c r="J181" s="25">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K181">
+      <c r="K181" s="25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L181">
+      <c r="L181" s="25">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M181" t="b">
+      <c r="M181" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -27348,7 +27397,7 @@
         <f t="shared" si="10"/>
         <v>67</v>
       </c>
-      <c r="M182" t="b">
+      <c r="M182" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27375,7 +27424,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M183" t="b">
+      <c r="M183" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27402,7 +27451,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M184" t="b">
+      <c r="M184" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27426,7 +27475,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M185" t="b">
+      <c r="M185" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27450,7 +27499,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M186" t="b">
+      <c r="M186" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27468,19 +27517,19 @@
       <c r="I187" s="16">
         <v>2200</v>
       </c>
-      <c r="J187">
+      <c r="J187" s="25">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K187">
+      <c r="K187" s="25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L187">
+      <c r="L187" s="25">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M187" t="b">
+      <c r="M187" s="12" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
@@ -27504,7 +27553,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M188" t="b">
+      <c r="M188" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27549,7 +27598,7 @@
         <f t="shared" si="10"/>
         <v>-5861</v>
       </c>
-      <c r="M189" t="b">
+      <c r="M189" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27573,7 +27622,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M190" t="b">
+      <c r="M190" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27597,7 +27646,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M191" t="b">
+      <c r="M191" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27624,7 +27673,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M192" t="b">
+      <c r="M192" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27660,7 +27709,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M193" t="b">
+      <c r="M193" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27684,7 +27733,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M194" t="b">
+      <c r="M194" s="12" t="b">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -27711,7 +27760,7 @@
         <f t="shared" ref="L195:L233" si="14">IF(AND(E195&gt;0,I195&gt;0),I195-E195,0)</f>
         <v>0</v>
       </c>
-      <c r="M195" t="b">
+      <c r="M195" s="12" t="b">
         <f t="shared" ref="M195:M233" si="15">IF(G195&gt;H195,TRUE,FALSE)</f>
         <v>0</v>
       </c>
@@ -27741,7 +27790,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M196" t="b">
+      <c r="M196" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -27759,19 +27808,19 @@
       <c r="I197" s="16">
         <v>3200</v>
       </c>
-      <c r="J197">
+      <c r="J197" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K197">
+      <c r="K197" s="25">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L197">
+      <c r="L197" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M197" t="b">
+      <c r="M197" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -27789,19 +27838,19 @@
       <c r="I198" s="16">
         <v>4100</v>
       </c>
-      <c r="J198">
+      <c r="J198" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K198">
+      <c r="K198" s="25">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L198">
+      <c r="L198" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M198" t="b">
+      <c r="M198" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -27846,7 +27895,7 @@
         <f t="shared" si="14"/>
         <v>-400</v>
       </c>
-      <c r="M199" t="b">
+      <c r="M199" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -27876,7 +27925,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M200" t="b">
+      <c r="M200" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -27894,19 +27943,19 @@
       <c r="I201" s="16">
         <v>1950</v>
       </c>
-      <c r="J201">
+      <c r="J201" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K201">
+      <c r="K201" s="25">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L201">
+      <c r="L201" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M201" t="b">
+      <c r="M201" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -27933,7 +27982,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M202" t="b">
+      <c r="M202" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -27957,7 +28006,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M203" t="b">
+      <c r="M203" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -27981,7 +28030,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M204" t="b">
+      <c r="M204" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28026,7 +28075,7 @@
         <f t="shared" si="14"/>
         <v>-4025</v>
       </c>
-      <c r="M205" t="b">
+      <c r="M205" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28056,7 +28105,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M206" t="b">
+      <c r="M206" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28092,7 +28141,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M207" t="b">
+      <c r="M207" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28122,7 +28171,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M208" t="b">
+      <c r="M208" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28140,19 +28189,19 @@
       <c r="I209" s="16">
         <v>1995</v>
       </c>
-      <c r="J209">
+      <c r="J209" s="11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K209">
+      <c r="K209" s="11">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L209">
+      <c r="L209" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M209" t="b">
+      <c r="M209" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -28182,7 +28231,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M210" t="b">
+      <c r="M210" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28212,7 +28261,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M211" t="b">
+      <c r="M211" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28230,19 +28279,19 @@
       <c r="I212" s="16">
         <v>1983</v>
       </c>
-      <c r="J212">
+      <c r="J212" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K212">
+      <c r="K212" s="25">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L212">
+      <c r="L212" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M212" t="b">
+      <c r="M212" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -28269,7 +28318,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M213" t="b">
+      <c r="M213" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28299,7 +28348,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M214" t="b">
+      <c r="M214" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28317,19 +28366,19 @@
       <c r="I215" s="16">
         <v>1800</v>
       </c>
-      <c r="J215">
+      <c r="J215" s="11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K215">
+      <c r="K215" s="11">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L215">
+      <c r="L215" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M215" t="b">
+      <c r="M215" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -28362,19 +28411,19 @@
       <c r="I216" s="16">
         <v>2163</v>
       </c>
-      <c r="J216">
+      <c r="J216" s="11">
         <f t="shared" si="12"/>
         <v>-41</v>
       </c>
-      <c r="K216">
+      <c r="K216" s="11">
         <f t="shared" si="13"/>
         <v>-264</v>
       </c>
-      <c r="L216">
+      <c r="L216" s="11">
         <f t="shared" si="14"/>
         <v>-262</v>
       </c>
-      <c r="M216" t="b">
+      <c r="M216" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -28401,7 +28450,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M217" t="b">
+      <c r="M217" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28428,7 +28477,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M218" t="b">
+      <c r="M218" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28458,7 +28507,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M219" t="b">
+      <c r="M219" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28503,7 +28552,7 @@
         <f t="shared" si="14"/>
         <v>-2031</v>
       </c>
-      <c r="M220" t="b">
+      <c r="M220" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28521,19 +28570,19 @@
       <c r="I221" s="16">
         <v>1725</v>
       </c>
-      <c r="J221">
+      <c r="J221" s="25">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K221">
+      <c r="K221" s="25">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L221">
+      <c r="L221" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M221" t="b">
+      <c r="M221" s="12" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
@@ -28560,7 +28609,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M222" t="b">
+      <c r="M222" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28587,7 +28636,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M223" t="b">
+      <c r="M223" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28614,7 +28663,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M224" t="b">
+      <c r="M224" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28659,7 +28708,7 @@
         <f t="shared" si="14"/>
         <v>-1459</v>
       </c>
-      <c r="M225" t="b">
+      <c r="M225" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28686,7 +28735,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M226" t="b">
+      <c r="M226" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28731,7 +28780,7 @@
         <f t="shared" si="14"/>
         <v>75</v>
       </c>
-      <c r="M227" t="b">
+      <c r="M227" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28761,7 +28810,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M228" t="b">
+      <c r="M228" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28788,7 +28837,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M229" t="b">
+      <c r="M229" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28812,7 +28861,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M230" t="b">
+      <c r="M230" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28842,7 +28891,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M231" t="b">
+      <c r="M231" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28866,7 +28915,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M232" t="b">
+      <c r="M232" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28902,7 +28951,7 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M233" t="b">
+      <c r="M233" s="12" t="b">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -28910,7 +28959,7 @@
     <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C234" s="11">
         <f>AVERAGE(C2:C233)</f>
-        <v>2301.7857142857142</v>
+        <v>2525.4363636363637</v>
       </c>
       <c r="D234" s="11">
         <f t="shared" ref="D234:I234" si="16">AVERAGE(D2:D233)</f>
@@ -28922,7 +28971,7 @@
       </c>
       <c r="F234" s="11">
         <f t="shared" si="16"/>
-        <v>7511.0892857142853</v>
+        <v>7829.454545454545</v>
       </c>
       <c r="G234" s="11">
         <f t="shared" si="16"/>
@@ -28938,7 +28987,7 @@
       </c>
       <c r="J234">
         <f t="shared" si="12"/>
-        <v>-284.71325051759823</v>
+        <v>-508.3638998682477</v>
       </c>
       <c r="N234" t="s">
         <v>577</v>
@@ -28959,7 +29008,7 @@
     <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G235">
         <f>(C234-G234)/(C234+G234)</f>
-        <v>6.5923269248423469E-2</v>
+        <v>0.11191258381301135</v>
       </c>
       <c r="H235">
         <f>(D234-H234)/(D234+H234)</f>
@@ -29051,6 +29100,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M2:M233">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -29059,8 +29119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67C7EEE-B502-4DC4-88E6-0F54EF23ECE1}">
   <dimension ref="A1:P330"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="L248" sqref="L248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29143,7 +29203,7 @@
         <v>40.865788000000002</v>
       </c>
       <c r="G2" s="12" t="b">
-        <f>IF(A2=H2,TRUE,FALSE)</f>
+        <f t="shared" ref="G2:G20" si="0">IF(A2=H2,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H2" t="s">
@@ -29183,7 +29243,7 @@
         <v>40.538114</v>
       </c>
       <c r="G3" s="12" t="b">
-        <f>IF(A3=H3,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H3" t="s">
@@ -29219,7 +29279,7 @@
         <v>40.549286000000002</v>
       </c>
       <c r="G4" s="12" t="b">
-        <f>IF(A4=H4,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4" t="s">
@@ -29255,7 +29315,7 @@
         <v>40.635325000000002</v>
       </c>
       <c r="G5" s="12" t="b">
-        <f>IF(A5=H5,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5" t="s">
@@ -29289,7 +29349,7 @@
         <v>40.596313000000002</v>
       </c>
       <c r="G6" s="12" t="b">
-        <f>IF(A6=H6,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6" t="s">
@@ -29323,7 +29383,7 @@
         <v>40.589143999999997</v>
       </c>
       <c r="G7" s="12" t="b">
-        <f>IF(A7=H7,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H7" t="s">
@@ -29357,7 +29417,7 @@
         <v>40.768509000000002</v>
       </c>
       <c r="G8" s="12" t="b">
-        <f>IF(A8=H8,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H8" t="s">
@@ -29397,7 +29457,7 @@
         <v>40.770316999999999</v>
       </c>
       <c r="G9" s="12" t="b">
-        <f>IF(A9=H9,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H9" t="s">
@@ -29431,7 +29491,7 @@
         <v>40.76173</v>
       </c>
       <c r="G10" s="12" t="b">
-        <f>IF(A10=H10,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H10" t="s">
@@ -29471,7 +29531,7 @@
         <v>40.599519000000001</v>
       </c>
       <c r="G11" s="12" t="b">
-        <f>IF(A11=H11,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H11" t="s">
@@ -29511,7 +29571,7 @@
         <v>40.711931999999997</v>
       </c>
       <c r="G12" s="12" t="b">
-        <f>IF(A12=H12,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H12" t="s">
@@ -29559,7 +29619,7 @@
         <v>40.625801000000003</v>
       </c>
       <c r="G13" s="12" t="b">
-        <f>IF(A13=H13,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" t="s">
@@ -29599,7 +29659,7 @@
         <v>40.782843</v>
       </c>
       <c r="G14" s="12" t="b">
-        <f>IF(A14=H14,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H14" t="s">
@@ -29633,7 +29693,7 @@
         <v>40.553987999999997</v>
       </c>
       <c r="G15" s="12" t="b">
-        <f>IF(A15=H15,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H15" t="s">
@@ -29667,7 +29727,7 @@
         <v>40.866858000000001</v>
       </c>
       <c r="G16" s="12" t="b">
-        <f>IF(A16=H16,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H16" t="s">
@@ -29701,7 +29761,7 @@
         <v>40.766041000000001</v>
       </c>
       <c r="G17" s="12" t="b">
-        <f>IF(A17=H17,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H17" t="s">
@@ -29741,7 +29801,7 @@
         <v>40.611322000000001</v>
       </c>
       <c r="G18" s="12" t="b">
-        <f>IF(A18=H18,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H18" t="s">
@@ -29775,7 +29835,7 @@
         <v>40.870184999999999</v>
       </c>
       <c r="G19" s="12" t="b">
-        <f>IF(A19=H19,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H19" t="s">
@@ -29815,7 +29875,7 @@
         <v>40.687232000000002</v>
       </c>
       <c r="G20" s="12" t="b">
-        <f>IF(A20=H20,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H20" t="s">
@@ -29887,7 +29947,7 @@
         <v>40.753385000000002</v>
       </c>
       <c r="G22" s="12" t="b">
-        <f>IF(A22=H22,TRUE,FALSE)</f>
+        <f t="shared" ref="G22:G32" si="1">IF(A22=H22,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H22" t="s">
@@ -29929,7 +29989,7 @@
         <v>40.733013999999997</v>
       </c>
       <c r="G23" s="12" t="b">
-        <f>IF(A23=H23,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H23" t="s">
@@ -29963,7 +30023,7 @@
         <v>40.576155999999997</v>
       </c>
       <c r="G24" s="12" t="b">
-        <f>IF(A24=H24,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H24" t="s">
@@ -29997,7 +30057,7 @@
         <v>40.728572999999997</v>
       </c>
       <c r="G25" s="12" t="b">
-        <f>IF(A25=H25,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H25" t="s">
@@ -30035,7 +30095,7 @@
         <v>40.857277000000003</v>
       </c>
       <c r="G26" s="12" t="b">
-        <f>IF(A26=H26,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H26" t="s">
@@ -30073,7 +30133,7 @@
         <v>40.611009000000003</v>
       </c>
       <c r="G27" s="12" t="b">
-        <f>IF(A27=H27,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H27" t="s">
@@ -30113,7 +30173,7 @@
         <v>40.61515</v>
       </c>
       <c r="G28" s="12" t="b">
-        <f>IF(A28=H28,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H28" t="s">
@@ -30151,7 +30211,7 @@
         <v>40.737251000000001</v>
       </c>
       <c r="G29" s="12" t="b">
-        <f>IF(A29=H29,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H29" t="s">
@@ -30189,7 +30249,7 @@
         <v>40.605778999999998</v>
       </c>
       <c r="G30" s="12" t="b">
-        <f>IF(A30=H30,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H30" t="s">
@@ -30223,7 +30283,7 @@
         <v>40.685682999999997</v>
       </c>
       <c r="G31" s="12" t="b">
-        <f>IF(A31=H31,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H31" t="s">
@@ -30271,7 +30331,7 @@
         <v>40.633130999999999</v>
       </c>
       <c r="G32" s="12" t="b">
-        <f>IF(A32=H32,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H32" t="s">
@@ -30410,7 +30470,7 @@
         <v>40.710934999999999</v>
       </c>
       <c r="G36" s="12" t="b">
-        <f>IF(A36=H36,TRUE,FALSE)</f>
+        <f t="shared" ref="G36:G53" si="2">IF(A36=H36,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H36" t="s">
@@ -30450,7 +30510,7 @@
         <v>40.576824999999999</v>
       </c>
       <c r="G37" s="12" t="b">
-        <f>IF(A37=H37,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H37" t="s">
@@ -30490,7 +30550,7 @@
         <v>40.603026999999997</v>
       </c>
       <c r="G38" s="12" t="b">
-        <f>IF(A38=H38,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H38" t="s">
@@ -30524,7 +30584,7 @@
         <v>40.677861</v>
       </c>
       <c r="G39" s="12" t="b">
-        <f>IF(A39=H39,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H39" t="s">
@@ -30558,7 +30618,7 @@
         <v>40.852722999999997</v>
       </c>
       <c r="G40" s="12" t="b">
-        <f>IF(A40=H40,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H40" t="s">
@@ -30592,7 +30652,7 @@
         <v>40.695864</v>
       </c>
       <c r="G41" s="12" t="b">
-        <f>IF(A41=H41,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H41" t="s">
@@ -30637,7 +30697,7 @@
         <v>40.702086999999999</v>
       </c>
       <c r="G42" s="12" t="b">
-        <f>IF(A42=H42,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H42" t="s">
@@ -30677,7 +30737,7 @@
         <v>40.660003000000003</v>
       </c>
       <c r="G43" s="12" t="b">
-        <f>IF(A43=H43,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H43" t="s">
@@ -30713,7 +30773,7 @@
         <v>40.66395</v>
       </c>
       <c r="G44" s="12" t="b">
-        <f>IF(A44=H44,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H44" t="s">
@@ -30753,7 +30813,7 @@
         <v>40.609591999999999</v>
       </c>
       <c r="G45" s="12" t="b">
-        <f>IF(A45=H45,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H45" t="s">
@@ -30791,7 +30851,7 @@
         <v>40.698115999999999</v>
       </c>
       <c r="G46" s="12" t="b">
-        <f>IF(A46=H46,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H46" t="s">
@@ -30839,7 +30899,7 @@
         <v>40.506081999999999</v>
       </c>
       <c r="G47" s="12" t="b">
-        <f>IF(A47=H47,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H47" t="s">
@@ -30873,7 +30933,7 @@
         <v>40.692774999999997</v>
       </c>
       <c r="G48" s="12" t="b">
-        <f>IF(A48=H48,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H48" t="s">
@@ -30907,7 +30967,7 @@
         <v>40.635564000000002</v>
       </c>
       <c r="G49" s="12" t="b">
-        <f>IF(A49=H49,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H49" t="s">
@@ -30947,7 +31007,7 @@
         <v>40.782682999999999</v>
       </c>
       <c r="G50" s="12" t="b">
-        <f>IF(A50=H50,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H50" t="s">
@@ -30989,7 +31049,7 @@
         <v>40.680540000000001</v>
       </c>
       <c r="G51" s="12" t="b">
-        <f>IF(A51=H51,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H51" t="s">
@@ -31037,7 +31097,7 @@
         <v>40.819014000000003</v>
       </c>
       <c r="G52" s="12" t="b">
-        <f>IF(A52=H52,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H52" t="s">
@@ -31073,7 +31133,7 @@
         <v>40.613335999999997</v>
       </c>
       <c r="G53" s="12" t="b">
-        <f>IF(A53=H53,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H53" t="s">
@@ -31613,7 +31673,7 @@
         <v>40.693229000000002</v>
       </c>
       <c r="G68" s="12" t="b">
-        <f>IF(A68=H68,TRUE,FALSE)</f>
+        <f t="shared" ref="G68:G76" si="3">IF(A68=H68,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H68" t="s">
@@ -31661,7 +31721,7 @@
         <v>40.687919999999998</v>
       </c>
       <c r="G69" s="12" t="b">
-        <f>IF(A69=H69,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H69" t="s">
@@ -31709,7 +31769,7 @@
         <v>40.784903</v>
       </c>
       <c r="G70" s="12" t="b">
-        <f>IF(A70=H70,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H70" t="s">
@@ -31747,7 +31807,7 @@
         <v>40.604472999999999</v>
       </c>
       <c r="G71" s="12" t="b">
-        <f>IF(A71=H71,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H71" t="s">
@@ -31785,7 +31845,7 @@
         <v>40.834283999999997</v>
       </c>
       <c r="G72" s="12" t="b">
-        <f>IF(A72=H72,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H72" t="s">
@@ -31825,7 +31885,7 @@
         <v>40.824779999999997</v>
       </c>
       <c r="G73" s="12" t="b">
-        <f>IF(A73=H73,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H73" t="s">
@@ -31865,7 +31925,7 @@
         <v>40.574292999999997</v>
       </c>
       <c r="G74" s="12" t="b">
-        <f>IF(A74=H74,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H74" t="s">
@@ -31905,7 +31965,7 @@
         <v>40.874293999999999</v>
       </c>
       <c r="G75" s="12" t="b">
-        <f>IF(A75=H75,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H75" t="s">
@@ -31941,7 +32001,7 @@
         <v>40.742381999999999</v>
       </c>
       <c r="G76" s="12" t="b">
-        <f>IF(A76=H76,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H76" t="s">
@@ -32281,7 +32341,7 @@
         <v>40.703175999999999</v>
       </c>
       <c r="G85" s="12" t="b">
-        <f>IF(A85=H85,TRUE,FALSE)</f>
+        <f t="shared" ref="G85:G92" si="4">IF(A85=H85,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H85" t="s">
@@ -32329,7 +32389,7 @@
         <v>40.619219000000001</v>
       </c>
       <c r="G86" s="12" t="b">
-        <f>IF(A86=H86,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H86" t="s">
@@ -32369,7 +32429,7 @@
         <v>40.764073000000003</v>
       </c>
       <c r="G87" s="12" t="b">
-        <f>IF(A87=H87,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H87" t="s">
@@ -32407,7 +32467,7 @@
         <v>40.641717999999997</v>
       </c>
       <c r="G88" s="12" t="b">
-        <f>IF(A88=H88,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H88" t="s">
@@ -32447,7 +32507,7 @@
         <v>40.792248999999998</v>
       </c>
       <c r="G89" s="12" t="b">
-        <f>IF(A89=H89,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H89" t="s">
@@ -32495,7 +32555,7 @@
         <v>40.669925999999997</v>
       </c>
       <c r="G90" s="12" t="b">
-        <f>IF(A90=H90,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H90" t="s">
@@ -32535,7 +32595,7 @@
         <v>40.842695999999997</v>
       </c>
       <c r="G91" s="12" t="b">
-        <f>IF(A91=H91,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H91" t="s">
@@ -32571,7 +32631,7 @@
         <v>40.727846999999997</v>
       </c>
       <c r="G92" s="12" t="b">
-        <f>IF(A92=H92,TRUE,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H92" t="s">
@@ -33655,7 +33715,7 @@
         <v>40.590848000000001</v>
       </c>
       <c r="G123" s="12" t="b">
-        <f>IF(A123=H123,TRUE,FALSE)</f>
+        <f t="shared" ref="G123:G129" si="5">IF(A123=H123,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H123" t="s">
@@ -33691,7 +33751,7 @@
         <v>40.749440999999997</v>
       </c>
       <c r="G124" s="12" t="b">
-        <f>IF(A124=H124,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H124" t="s">
@@ -33729,7 +33789,7 @@
         <v>40.702762</v>
       </c>
       <c r="G125" s="12" t="b">
-        <f>IF(A125=H125,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H125" t="s">
@@ -33769,7 +33829,7 @@
         <v>40.673931000000003</v>
       </c>
       <c r="G126" s="12" t="b">
-        <f>IF(A126=H126,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H126" t="s">
@@ -33817,7 +33877,7 @@
         <v>40.737209999999997</v>
       </c>
       <c r="G127" s="12" t="b">
-        <f>IF(A127=H127,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H127" t="s">
@@ -33865,7 +33925,7 @@
         <v>40.620171999999997</v>
       </c>
       <c r="G128" s="12" t="b">
-        <f>IF(A128=H128,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H128" t="s">
@@ -33901,7 +33961,7 @@
         <v>40.576216000000002</v>
       </c>
       <c r="G129" s="12" t="b">
-        <f>IF(A129=H129,TRUE,FALSE)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H129" t="s">
@@ -34736,7 +34796,7 @@
         <v>40.809730000000002</v>
       </c>
       <c r="G153" s="12" t="b">
-        <f>IF(A153=H153,TRUE,FALSE)</f>
+        <f t="shared" ref="G153:G162" si="6">IF(A153=H153,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H153" t="s">
@@ -34774,7 +34834,7 @@
         <v>40.867683999999997</v>
       </c>
       <c r="G154" s="12" t="b">
-        <f>IF(A154=H154,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H154" t="s">
@@ -34822,7 +34882,7 @@
         <v>40.751981000000001</v>
       </c>
       <c r="G155" s="12" t="b">
-        <f>IF(A155=H155,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H155" t="s">
@@ -34862,7 +34922,7 @@
         <v>40.704656999999997</v>
       </c>
       <c r="G156" s="12" t="b">
-        <f>IF(A156=H156,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H156" t="s">
@@ -34902,7 +34962,7 @@
         <v>40.716805000000001</v>
       </c>
       <c r="G157" s="12" t="b">
-        <f>IF(A157=H157,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H157" t="s">
@@ -34942,7 +35002,7 @@
         <v>40.711460000000002</v>
       </c>
       <c r="G158" s="12" t="b">
-        <f>IF(A158=H158,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H158" t="s">
@@ -34982,7 +35042,7 @@
         <v>40.642381999999998</v>
       </c>
       <c r="G159" s="12" t="b">
-        <f>IF(A159=H159,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H159" t="s">
@@ -35030,7 +35090,7 @@
         <v>40.705179000000001</v>
       </c>
       <c r="G160" s="12" t="b">
-        <f>IF(A160=H160,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H160" t="s">
@@ -35070,7 +35130,7 @@
         <v>40.722577999999999</v>
       </c>
       <c r="G161" s="12" t="b">
-        <f>IF(A161=H161,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H161" t="s">
@@ -35110,7 +35170,7 @@
         <v>40.881686999999999</v>
       </c>
       <c r="G162" s="12" t="b">
-        <f>IF(A162=H162,TRUE,FALSE)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H162" t="s">
@@ -36362,7 +36422,7 @@
         <v>40.808</v>
       </c>
       <c r="G197" s="12" t="b">
-        <f>IF(A197=H197,TRUE,FALSE)</f>
+        <f t="shared" ref="G197:G204" si="7">IF(A197=H197,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H197" t="s">
@@ -36404,7 +36464,7 @@
         <v>40.847898000000001</v>
       </c>
       <c r="G198" s="12" t="b">
-        <f>IF(A198=H198,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H198" t="s">
@@ -36444,7 +36504,7 @@
         <v>40.847549000000001</v>
       </c>
       <c r="G199" s="12" t="b">
-        <f>IF(A199=H199,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H199" t="s">
@@ -36484,7 +36544,7 @@
         <v>40.823591999999998</v>
       </c>
       <c r="G200" s="12" t="b">
-        <f>IF(A200=H200,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H200" t="s">
@@ -36520,7 +36580,7 @@
         <v>40.806238999999998</v>
       </c>
       <c r="G201" s="12" t="b">
-        <f>IF(A201=H201,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H201" t="s">
@@ -36560,7 +36620,7 @@
         <v>40.843826</v>
       </c>
       <c r="G202" s="12" t="b">
-        <f>IF(A202=H202,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H202" t="s">
@@ -36600,7 +36660,7 @@
         <v>40.848841999999998</v>
       </c>
       <c r="G203" s="12" t="b">
-        <f>IF(A203=H203,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H203" t="s">
@@ -36640,7 +36700,7 @@
         <v>40.748303</v>
       </c>
       <c r="G204" s="12" t="b">
-        <f>IF(A204=H204,TRUE,FALSE)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="H204" t="s">
@@ -37448,7 +37508,7 @@
         <v>40.672320999999997</v>
       </c>
       <c r="G228" s="12" t="b">
-        <f>IF(A228=H228,TRUE,FALSE)</f>
+        <f t="shared" ref="G228:G233" si="8">IF(A228=H228,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H228" t="s">
@@ -37496,7 +37556,7 @@
         <v>40.837938000000001</v>
       </c>
       <c r="G229" s="12" t="b">
-        <f>IF(A229=H229,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H229" t="s">
@@ -37533,7 +37593,7 @@
         <v>40.773673000000002</v>
       </c>
       <c r="G230" s="12" t="b">
-        <f>IF(A230=H230,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H230" t="s">
@@ -37575,7 +37635,7 @@
         <v>40.850641000000003</v>
       </c>
       <c r="G231" s="12" t="b">
-        <f>IF(A231=H231,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H231" t="s">
@@ -37615,7 +37675,7 @@
         <v>40.862966</v>
       </c>
       <c r="G232" s="12" t="b">
-        <f>IF(A232=H232,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H232" t="s">
@@ -37651,7 +37711,7 @@
         <v>40.857413000000001</v>
       </c>
       <c r="G233" s="12" t="b">
-        <f>IF(A233=H233,TRUE,FALSE)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H233" t="s">
@@ -38153,18 +38213,14 @@
       <c r="H248" t="s">
         <v>155</v>
       </c>
-      <c r="I248" s="12">
-        <v>-9999</v>
-      </c>
+      <c r="I248" s="12"/>
       <c r="J248" s="15">
         <v>2300</v>
       </c>
       <c r="K248" s="16">
         <v>4287</v>
       </c>
-      <c r="L248" s="13">
-        <v>-9999</v>
-      </c>
+      <c r="L248" s="13"/>
       <c r="M248" s="12">
         <v>1673</v>
       </c>
@@ -40626,7 +40682,7 @@
         <v>40.621090000000002</v>
       </c>
       <c r="G318" s="12" t="b">
-        <f>IF(A318=H318,TRUE,FALSE)</f>
+        <f t="shared" ref="G318:G323" si="9">IF(A318=H318,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H318" t="s">
@@ -40664,7 +40720,7 @@
         <v>40.781291000000003</v>
       </c>
       <c r="G319" s="12" t="b">
-        <f>IF(A319=H319,TRUE,FALSE)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H319" t="s">
@@ -40702,7 +40758,7 @@
         <v>40.881039000000001</v>
       </c>
       <c r="G320" s="12" t="b">
-        <f>IF(A320=H320,TRUE,FALSE)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H320" t="s">
@@ -40740,7 +40796,7 @@
         <v>40.707144</v>
       </c>
       <c r="G321" s="12" t="b">
-        <f>IF(A321=H321,TRUE,FALSE)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H321" t="s">
@@ -40788,7 +40844,7 @@
         <v>40.603707</v>
       </c>
       <c r="G322" s="12" t="b">
-        <f>IF(A322=H322,TRUE,FALSE)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H322" t="s">
@@ -40826,7 +40882,7 @@
         <v>40.656945999999998</v>
       </c>
       <c r="G323" s="12" t="b">
-        <f>IF(A323=H323,TRUE,FALSE)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H323" t="s">
@@ -40901,7 +40957,7 @@
         <v>40.689886999999999</v>
       </c>
       <c r="G325" s="12" t="b">
-        <f>IF(A325=H325,TRUE,FALSE)</f>
+        <f t="shared" ref="G325:G330" si="10">IF(A325=H325,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H325" t="s">
@@ -40941,7 +40997,7 @@
         <v>40.898273000000003</v>
       </c>
       <c r="G326" s="12" t="b">
-        <f>IF(A326=H326,TRUE,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H326" t="s">
@@ -40979,7 +41035,7 @@
         <v>40.541967999999997</v>
       </c>
       <c r="G327" s="12" t="b">
-        <f>IF(A327=H327,TRUE,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H327" t="s">
@@ -41015,7 +41071,7 @@
         <v>40.746349000000002</v>
       </c>
       <c r="G328" s="12" t="b">
-        <f>IF(A328=H328,TRUE,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H328" t="s">
@@ -41052,7 +41108,7 @@
         <v>40.817444999999999</v>
       </c>
       <c r="G329" s="12" t="b">
-        <f>IF(A329=H329,TRUE,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H329" t="s">
@@ -41088,7 +41144,7 @@
         <v>40.775930000000002</v>
       </c>
       <c r="G330" s="12" t="b">
-        <f>IF(A330=H330,TRUE,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H330" t="s">
@@ -41112,13 +41168,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41130,8 +41186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3543610-9771-4F3E-B476-241AAB624B73}">
   <dimension ref="A1:M330"/>
   <sheetViews>
-    <sheetView topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="P250" sqref="P250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -48931,18 +48987,14 @@
       <c r="F248">
         <v>40.676253000000003</v>
       </c>
-      <c r="G248" s="12">
-        <v>-9999</v>
-      </c>
+      <c r="G248" s="12"/>
       <c r="H248" s="15">
         <v>2300</v>
       </c>
       <c r="I248" s="16">
         <v>4287</v>
       </c>
-      <c r="J248" s="13">
-        <v>-9999</v>
-      </c>
+      <c r="J248" s="13"/>
       <c r="K248" s="12">
         <v>1673</v>
       </c>

</xml_diff>

<commit_message>
Fixed bad coordinate data for South Slope
</commit_message>
<xml_diff>
--- a/data/nyc_data_join.xlsx
+++ b/data/nyc_data_join.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64426d83357dbd62/LHL/_DataScienciBootCamp/Midterm_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2536" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC9D83F-8C59-42FB-85F4-44C147C5910D}"/>
+  <xr:revisionPtr revIDLastSave="2542" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E60D2566-E81D-4EBE-A1CA-DC21BB814E4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{C1537D77-E0D5-2B49-9CF0-C1029E12ACBF}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5454" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5454" uniqueCount="1050">
   <si>
     <t>Astoria</t>
   </si>
@@ -3121,9 +3121,6 @@
   </si>
   <si>
     <t>South Side is NOT South Slope</t>
-  </si>
-  <si>
-    <t>Bronx?</t>
   </si>
   <si>
     <t>Fort Hamilton === Fort Wadsworth</t>
@@ -21687,7 +21684,7 @@
         <v>590</v>
       </c>
       <c r="M1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -29167,15 +29164,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67C7EEE-B502-4DC4-88E6-0F54EF23ECE1}">
   <dimension ref="A1:P330"/>
   <sheetViews>
-    <sheetView topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="E279" sqref="E279:F279"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
@@ -29983,7 +29980,7 @@
         <v>479</v>
       </c>
       <c r="B22" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -30434,7 +30431,7 @@
         <v>506</v>
       </c>
       <c r="B34" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -30476,7 +30473,7 @@
         <v>187</v>
       </c>
       <c r="B35" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -30742,7 +30739,7 @@
         <v>318</v>
       </c>
       <c r="B42" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -31256,7 +31253,7 @@
         <v>2400</v>
       </c>
       <c r="P54" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -31264,7 +31261,7 @@
         <v>277</v>
       </c>
       <c r="B55" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
@@ -31631,7 +31628,7 @@
         <v>410</v>
       </c>
       <c r="B65" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C65" t="s">
         <v>47</v>
@@ -32092,10 +32089,10 @@
         <v>427</v>
       </c>
       <c r="B77" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C77" t="s">
-        <v>1023</v>
+        <v>64</v>
       </c>
       <c r="E77">
         <v>40.836559999999999</v>
@@ -33568,7 +33565,7 @@
         <v>5595</v>
       </c>
       <c r="P116" s="11" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -33576,10 +33573,10 @@
         <v>314</v>
       </c>
       <c r="B117" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C117" t="s">
-        <v>1023</v>
+        <v>64</v>
       </c>
       <c r="D117" t="s">
         <v>596</v>
@@ -33708,7 +33705,7 @@
         <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
@@ -34285,7 +34282,7 @@
         <v>210</v>
       </c>
       <c r="B136" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C136" t="s">
         <v>3</v>
@@ -34430,7 +34427,7 @@
         <v>24</v>
       </c>
       <c r="B140" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C140" t="s">
         <v>34</v>
@@ -35303,7 +35300,7 @@
         <v>29</v>
       </c>
       <c r="B164" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C164" t="s">
         <v>34</v>
@@ -35343,7 +35340,7 @@
         <v>238</v>
       </c>
       <c r="B165" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C165" t="s">
         <v>34</v>
@@ -36013,7 +36010,7 @@
         <v>365</v>
       </c>
       <c r="B184" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C184" t="s">
         <v>3</v>
@@ -37091,7 +37088,7 @@
         <v>578</v>
       </c>
       <c r="B213" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C213" t="s">
         <v>34</v>
@@ -37175,7 +37172,7 @@
         <v>41</v>
       </c>
       <c r="B215" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C215" t="s">
         <v>34</v>
@@ -37677,7 +37674,7 @@
         <v>498</v>
       </c>
       <c r="B230" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C230" t="s">
         <v>34</v>
@@ -38572,7 +38569,7 @@
         <v>518</v>
       </c>
       <c r="B256" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C256" t="s">
         <v>34</v>
@@ -39366,7 +39363,7 @@
         <v>567</v>
       </c>
       <c r="B279" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C279" t="s">
         <v>3</v>
@@ -39811,7 +39808,7 @@
         <v>53</v>
       </c>
       <c r="B292" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C292" t="s">
         <v>34</v>
@@ -40164,7 +40161,7 @@
         <v>237</v>
       </c>
       <c r="B302" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C302" t="s">
         <v>34</v>
@@ -40388,10 +40385,10 @@
     </row>
     <row r="308" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B308" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C308" t="s">
         <v>64</v>
@@ -40407,7 +40404,7 @@
         <v>1</v>
       </c>
       <c r="H308" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I308" s="12"/>
       <c r="J308" s="15"/>
@@ -41210,7 +41207,7 @@
         <v>430</v>
       </c>
       <c r="B329" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C329" t="s">
         <v>64</v>
@@ -41303,15 +41300,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3543610-9771-4F3E-B476-241AAB624B73}">
   <dimension ref="A1:M330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="R280" sqref="R280"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
@@ -41981,7 +41978,7 @@
         <v>479</v>
       </c>
       <c r="B22" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -42355,7 +42352,7 @@
         <v>506</v>
       </c>
       <c r="B34" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -42390,7 +42387,7 @@
         <v>187</v>
       </c>
       <c r="B35" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -42608,7 +42605,7 @@
         <v>318</v>
       </c>
       <c r="B42" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -43037,7 +43034,7 @@
         <v>277</v>
       </c>
       <c r="B55" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
@@ -43356,7 +43353,7 @@
         <v>410</v>
       </c>
       <c r="B65" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C65" t="s">
         <v>47</v>
@@ -43748,10 +43745,10 @@
         <v>427</v>
       </c>
       <c r="B77" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C77" t="s">
-        <v>1023</v>
+        <v>64</v>
       </c>
       <c r="E77">
         <v>40.836559999999999</v>
@@ -45037,10 +45034,10 @@
         <v>314</v>
       </c>
       <c r="B117" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C117" t="s">
-        <v>1023</v>
+        <v>64</v>
       </c>
       <c r="D117" t="s">
         <v>596</v>
@@ -45155,7 +45152,7 @@
         <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C121" t="s">
         <v>34</v>
@@ -45648,7 +45645,7 @@
         <v>210</v>
       </c>
       <c r="B136" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C136" t="s">
         <v>3</v>
@@ -45772,7 +45769,7 @@
         <v>24</v>
       </c>
       <c r="B140" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="C140" t="s">
         <v>34</v>
@@ -46526,7 +46523,7 @@
         <v>29</v>
       </c>
       <c r="B164" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C164" t="s">
         <v>34</v>
@@ -46559,7 +46556,7 @@
         <v>238</v>
       </c>
       <c r="B165" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C165" t="s">
         <v>34</v>
@@ -47150,7 +47147,7 @@
         <v>365</v>
       </c>
       <c r="B184" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C184" t="s">
         <v>3</v>
@@ -48069,7 +48066,7 @@
         <v>578</v>
       </c>
       <c r="B213" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C213" t="s">
         <v>34</v>
@@ -48140,7 +48137,7 @@
         <v>41</v>
       </c>
       <c r="B215" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="C215" t="s">
         <v>34</v>
@@ -48593,7 +48590,7 @@
         <v>498</v>
       </c>
       <c r="B230" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C230" t="s">
         <v>34</v>
@@ -49391,7 +49388,7 @@
         <v>518</v>
       </c>
       <c r="B256" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C256" t="s">
         <v>34</v>
@@ -50084,7 +50081,7 @@
         <v>567</v>
       </c>
       <c r="B279" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C279" t="s">
         <v>3</v>
@@ -50481,7 +50478,7 @@
         <v>53</v>
       </c>
       <c r="B292" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C292" t="s">
         <v>34</v>
@@ -50793,7 +50790,7 @@
         <v>237</v>
       </c>
       <c r="B302" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C302" t="s">
         <v>34</v>
@@ -50982,10 +50979,10 @@
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B308" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C308" t="s">
         <v>64</v>
@@ -51675,7 +51672,7 @@
         <v>430</v>
       </c>
       <c r="B329" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C329" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
fixed bad lat long for Broadway
</commit_message>
<xml_diff>
--- a/data/nyc_data_join.xlsx
+++ b/data/nyc_data_join.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64426d83357dbd62/LHL/_DataScienciBootCamp/Midterm_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2542" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E60D2566-E81D-4EBE-A1CA-DC21BB814E4C}"/>
+  <xr:revisionPtr revIDLastSave="2563" documentId="8_{DEB721CE-31B5-47EA-9940-F813073CBCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04677F5D-E4CB-4AF8-ACED-463E6C6E7AEE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{C1537D77-E0D5-2B49-9CF0-C1029E12ACBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C1537D77-E0D5-2B49-9CF0-C1029E12ACBF}"/>
   </bookViews>
   <sheets>
     <sheet name="housing_prices" sheetId="2" r:id="rId1"/>
@@ -29164,8 +29164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67C7EEE-B502-4DC4-88E6-0F54EF23ECE1}">
   <dimension ref="A1:P330"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="P301" sqref="P301:S301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -30440,10 +30440,10 @@
         <v>596</v>
       </c>
       <c r="E34">
-        <v>40.812967999999998</v>
+        <v>40.812432999999999</v>
       </c>
       <c r="F34">
-        <v>-73.983159000000001</v>
+        <v>-73.960533999999996</v>
       </c>
       <c r="G34" s="12" t="b">
         <f>IF(A34=H34,TRUE,FALSE)</f>
@@ -41293,6 +41293,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -41300,8 +41301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3543610-9771-4F3E-B476-241AAB624B73}">
   <dimension ref="A1:M330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -41316,6 +41317,7 @@
     <col min="8" max="10" width="9.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -42361,10 +42363,10 @@
         <v>596</v>
       </c>
       <c r="E34">
-        <v>40.812967999999998</v>
+        <v>40.812432999999999</v>
       </c>
       <c r="F34">
-        <v>-73.983159000000001</v>
+        <v>-73.960533999999996</v>
       </c>
       <c r="G34" s="12">
         <v>2328</v>
@@ -51733,6 +51735,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>